<commit_message>
Getting all details as a dict
</commit_message>
<xml_diff>
--- a/Yelp_Results.xlsx
+++ b/Yelp_Results.xlsx
@@ -16,61 +16,61 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
-    <t>&lt;meta content="Get Off My Nerves Chiropractic - Baton Rouge, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Capital City Chiropractic - Baton Rouge, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Leist Chiropractic Clinic - Baker, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Zachary Chiropractic Clinic - Zachary, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Sonnier Chiropractic Clinic - Baton Rouge, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Louisiana Chiropractic - Port Allen, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Prewitt Chiropractic Clinic - Baker, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Ozark Chiropractic Clinic - Baton Rouge, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Spencer’s Chiropractic Clinic - Baton Rouge, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Community Chiropractic - Baton Rouge, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Chiro-Practical - Zachary, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Family Chiropractic Clinic - Baton Rouge, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Massage Emporium - Baton Rouge, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Core Chiropractic Clinic - Prairieville, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Underwood Chiropractic Clinic - Baton Rouge, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Family and Sports Chiropractic - Saint Francisville, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Spine and Sport Rehab Center - Baton Rouge, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Chiropractic Sports &amp;amp; Injury Center - Baton Rouge, LA" property="og:title"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta content="Capitol Spine and Rehabilitation - Baton Rouge, LA" property="og:title"/&gt;</t>
+    <t>Get Off My Nerves Chiropractic</t>
+  </si>
+  <si>
+    <t>Capital City Chiropractic</t>
+  </si>
+  <si>
+    <t>Leist Chiropractic Clinic</t>
+  </si>
+  <si>
+    <t>Zachary Chiropractic Clinic</t>
+  </si>
+  <si>
+    <t>Sonnier Chiropractic Clinic</t>
+  </si>
+  <si>
+    <t>Louisiana Chiropractic</t>
+  </si>
+  <si>
+    <t>Prewitt Chiropractic Clinic</t>
+  </si>
+  <si>
+    <t>Ozark Chiropractic Clinic</t>
+  </si>
+  <si>
+    <t>Spencer’s Chiropractic Clinic</t>
+  </si>
+  <si>
+    <t>Community Chiropractic</t>
+  </si>
+  <si>
+    <t>Chiro-Practical</t>
+  </si>
+  <si>
+    <t>Family Chiropractic Clinic</t>
+  </si>
+  <si>
+    <t>Massage Emporium</t>
+  </si>
+  <si>
+    <t>Core Chiropractic Clinic</t>
+  </si>
+  <si>
+    <t>Underwood Chiropractic Clinic</t>
+  </si>
+  <si>
+    <t>Family and Sports Chiropractic</t>
+  </si>
+  <si>
+    <t>Spine and Sport Rehab Center</t>
+  </si>
+  <si>
+    <t>Chiropractic Sports &amp; Injury Center</t>
+  </si>
+  <si>
+    <t>Capitol Spine and Rehabilitation</t>
   </si>
 </sst>
 </file>

</xml_diff>